<commit_message>
fixed some copper features
</commit_message>
<xml_diff>
--- a/master_worksheet.xlsx
+++ b/master_worksheet.xlsx
@@ -222,11 +222,19 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -237,14 +245,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,7 +528,7 @@
   <dimension ref="C2:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,18 +536,18 @@
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="9"/>
+    <col min="9" max="9" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
@@ -558,7 +558,7 @@
       </c>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D6" t="s">
@@ -579,7 +579,7 @@
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="1"/>
+      <c r="C7" s="6"/>
       <c r="D7" t="s">
         <v>3</v>
       </c>
@@ -598,10 +598,10 @@
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="2"/>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D9" t="s">
@@ -620,12 +620,12 @@
         <f>F9*G9</f>
         <v>8</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="3"/>
+      <c r="C10" s="7"/>
       <c r="D10" t="s">
         <v>2</v>
       </c>
@@ -644,7 +644,7 @@
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="3"/>
+      <c r="C11" s="7"/>
       <c r="D11" t="s">
         <v>12</v>
       </c>
@@ -663,7 +663,7 @@
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="3"/>
+      <c r="C12" s="7"/>
       <c r="E12" t="s">
         <v>18</v>
       </c>
@@ -679,10 +679,10 @@
       </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="2"/>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
@@ -703,7 +703,7 @@
       </c>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D16" t="s">
@@ -724,7 +724,7 @@
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="4"/>
+      <c r="C17" s="8"/>
       <c r="D17" t="s">
         <v>12</v>
       </c>
@@ -743,7 +743,7 @@
       </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="4"/>
+      <c r="C18" s="8"/>
       <c r="D18" t="s">
         <v>12</v>
       </c>
@@ -762,7 +762,7 @@
       </c>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C19" s="4"/>
+      <c r="C19" s="8"/>
       <c r="D19" t="s">
         <v>12</v>
       </c>
@@ -781,7 +781,7 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="4"/>
+      <c r="C20" s="8"/>
       <c r="D20" t="s">
         <v>21</v>
       </c>
@@ -800,7 +800,7 @@
       </c>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D22" t="s">
@@ -816,12 +816,12 @@
         <v>3</v>
       </c>
       <c r="H22">
-        <f>F22*G22</f>
+        <f t="shared" ref="H22:H28" si="0">F22*G22</f>
         <v>6</v>
       </c>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="5"/>
+      <c r="C23" s="9"/>
       <c r="D23" t="s">
         <v>12</v>
       </c>
@@ -835,12 +835,12 @@
         <v>3</v>
       </c>
       <c r="H23">
-        <f>F23*G23</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="5"/>
+      <c r="C24" s="9"/>
       <c r="D24" t="s">
         <v>12</v>
       </c>
@@ -854,12 +854,12 @@
         <v>1</v>
       </c>
       <c r="H24">
-        <f>F24*G24</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="5"/>
+      <c r="C25" s="9"/>
       <c r="D25" t="s">
         <v>12</v>
       </c>
@@ -873,12 +873,12 @@
         <v>1</v>
       </c>
       <c r="H25">
-        <f>F25*G25</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="5"/>
+      <c r="C26" s="9"/>
       <c r="D26" t="s">
         <v>12</v>
       </c>
@@ -892,12 +892,12 @@
         <v>1</v>
       </c>
       <c r="H26">
-        <f>F26*G26</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C27" s="5"/>
+      <c r="C27" s="9"/>
       <c r="D27" t="s">
         <v>12</v>
       </c>
@@ -911,12 +911,12 @@
         <v>1</v>
       </c>
       <c r="H27">
-        <f>F27*G27</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C28" s="5"/>
+      <c r="C28" s="9"/>
       <c r="D28" t="s">
         <v>12</v>
       </c>
@@ -930,12 +930,12 @@
         <v>1</v>
       </c>
       <c r="H28">
-        <f>F28*G28</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="H31" s="7"/>
+      <c r="H31" s="3"/>
     </row>
     <row r="32" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G32" t="s">

</xml_diff>